<commit_message>
Changed outputPeriodicalPayments to use pointers cause we were forced to #tyranny, also implemented bankers rounding.
Co-Authored-By: SimonCV <80058249+SimonCV@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/CLion/cppexercises/9.1_Laaneberegning/Assets/Renteberegning.xlsx
+++ b/CLion/cppexercises/9.1_Laaneberegning/Assets/Renteberegning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\CPP-Learning\CLion\cppexercises\9.1_Laaneberegning\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D8485C-8661-42A5-90DB-A5C82AED1200}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A21471-F5A7-4D93-96EA-F98E1145100D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-195" windowWidth="29040" windowHeight="15840" xr2:uid="{18E3E89E-692F-49DB-9FD0-C3C2968C172D}"/>
   </bookViews>
@@ -444,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D30B933-58E4-490D-B249-829C32543B81}">
-  <dimension ref="A1:L70"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -457,11 +457,11 @@
     <col min="6" max="8" width="9.140625" style="1"/>
     <col min="9" max="10" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="13" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,14 +483,14 @@
       <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -519,20 +519,20 @@
         <f>B1-H2</f>
         <v>986741.64477364614</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <f>B1-I2</f>
         <v>13258.355226353859</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <f>SUM(G2:G61)</f>
         <v>245501.31358124348</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <f>SUM(F2:F61)</f>
         <v>1245501.3135812292</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -558,12 +558,12 @@
         <f>I2-H3</f>
         <v>973383.85188309464</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <f>I2-I3</f>
         <v>13357.7928905515</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -590,12 +590,12 @@
         <f t="shared" ref="I4:I61" si="3">I3-H4</f>
         <v>959925.87554586399</v>
       </c>
-      <c r="J4" s="2">
-        <f t="shared" ref="J4:J24" si="4">I3-I4</f>
+      <c r="K4" s="2">
+        <f>I3-I4</f>
         <v>13457.976337230648</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -621,12 +621,12 @@
         <f t="shared" si="3"/>
         <v>946366.96438610414</v>
       </c>
-      <c r="J5" s="2">
-        <f t="shared" si="4"/>
+      <c r="K5" s="2">
+        <f>I4-I5</f>
         <v>13558.911159759853</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -653,12 +653,12 @@
         <f t="shared" si="3"/>
         <v>932706.3613926461</v>
       </c>
-      <c r="J6" s="2">
-        <f t="shared" si="4"/>
+      <c r="K6" s="2">
+        <f>I5-I6</f>
         <v>13660.602993458044</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E7" s="1">
         <v>6</v>
       </c>
@@ -678,12 +678,12 @@
         <f t="shared" si="3"/>
         <v>918943.30387673713</v>
       </c>
-      <c r="J7" s="2">
-        <f t="shared" si="4"/>
+      <c r="K7" s="2">
+        <f>I6-I7</f>
         <v>13763.057515908964</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E8" s="1">
         <v>7</v>
       </c>
@@ -703,12 +703,12 @@
         <f t="shared" si="3"/>
         <v>905077.02342945884</v>
       </c>
-      <c r="J8" s="2">
-        <f t="shared" si="4"/>
+      <c r="K8" s="2">
+        <f>I7-I8</f>
         <v>13866.280447278288</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E9" s="1">
         <v>8</v>
       </c>
@@ -728,12 +728,12 @@
         <f t="shared" si="3"/>
         <v>891106.74587882601</v>
       </c>
-      <c r="J9" s="2">
-        <f t="shared" si="4"/>
+      <c r="K9" s="2">
+        <f>I8-I9</f>
         <v>13970.277550632833</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E10" s="1">
         <v>9</v>
       </c>
@@ -753,12 +753,12 @@
         <f t="shared" si="3"/>
         <v>877031.69124656334</v>
       </c>
-      <c r="J10" s="2">
-        <f t="shared" si="4"/>
+      <c r="K10" s="2">
+        <f>I9-I10</f>
         <v>14075.054632262676</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E11" s="1">
         <v>10</v>
       </c>
@@ -778,12 +778,12 @@
         <f t="shared" si="3"/>
         <v>862851.07370455877</v>
       </c>
-      <c r="J11" s="2">
-        <f t="shared" si="4"/>
+      <c r="K11" s="2">
+        <f>I10-I11</f>
         <v>14180.617542004562</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E12" s="1">
         <v>11</v>
       </c>
@@ -803,12 +803,12 @@
         <f t="shared" si="3"/>
         <v>848564.10153098917</v>
       </c>
-      <c r="J12" s="2">
-        <f t="shared" si="4"/>
+      <c r="K12" s="2">
+        <f>I11-I12</f>
         <v>14286.972173569608</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E13" s="1">
         <v>12</v>
       </c>
@@ -828,12 +828,12 @@
         <f t="shared" si="3"/>
         <v>834169.9770661178</v>
       </c>
-      <c r="J13" s="2">
-        <f t="shared" si="4"/>
+      <c r="K13" s="2">
+        <f>I12-I13</f>
         <v>14394.124464871362</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E14" s="1">
         <v>13</v>
       </c>
@@ -853,12 +853,12 @@
         <f t="shared" si="3"/>
         <v>819667.89666775987</v>
       </c>
-      <c r="J14" s="2">
-        <f t="shared" si="4"/>
+      <c r="K14" s="2">
+        <f>I13-I14</f>
         <v>14502.080398357939</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E15" s="1">
         <v>14</v>
       </c>
@@ -878,12 +878,12 @@
         <f t="shared" si="3"/>
         <v>805057.0506664142</v>
       </c>
-      <c r="J15" s="2">
-        <f t="shared" si="4"/>
+      <c r="K15" s="2">
+        <f>I14-I15</f>
         <v>14610.846001345664</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E16" s="1">
         <v>15</v>
       </c>
@@ -903,12 +903,12 @@
         <f t="shared" si="3"/>
         <v>790336.62332005845</v>
       </c>
-      <c r="J16" s="2">
-        <f t="shared" si="4"/>
+      <c r="K16" s="2">
+        <f>I15-I16</f>
         <v>14720.427346355747</v>
       </c>
     </row>
-    <row r="17" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E17" s="1">
         <v>16</v>
       </c>
@@ -928,12 +928,12 @@
         <f t="shared" si="3"/>
         <v>775505.79276860505</v>
       </c>
-      <c r="J17" s="2">
-        <f t="shared" si="4"/>
+      <c r="K17" s="2">
+        <f>I16-I17</f>
         <v>14830.8305514534</v>
       </c>
     </row>
-    <row r="18" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E18" s="1">
         <v>17</v>
       </c>
@@ -953,12 +953,12 @@
         <f t="shared" si="3"/>
         <v>760563.73098801577</v>
       </c>
-      <c r="J18" s="2">
-        <f t="shared" si="4"/>
+      <c r="K18" s="2">
+        <f>I17-I18</f>
         <v>14942.061780589283</v>
       </c>
     </row>
-    <row r="19" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E19" s="1">
         <v>18</v>
       </c>
@@ -978,12 +978,12 @@
         <f t="shared" si="3"/>
         <v>745509.60374407202</v>
       </c>
-      <c r="J19" s="2">
-        <f t="shared" si="4"/>
+      <c r="K19" s="2">
+        <f>I18-I19</f>
         <v>15054.127243943745</v>
       </c>
     </row>
-    <row r="20" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E20" s="1">
         <v>19</v>
       </c>
@@ -1003,12 +1003,12 @@
         <f t="shared" si="3"/>
         <v>730342.57054579875</v>
       </c>
-      <c r="J20" s="2">
-        <f t="shared" si="4"/>
+      <c r="K20" s="2">
+        <f>I19-I20</f>
         <v>15167.033198273275</v>
       </c>
     </row>
-    <row r="21" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E21" s="1">
         <v>20</v>
       </c>
@@ -1028,12 +1028,12 @@
         <f t="shared" si="3"/>
         <v>715061.78459853842</v>
       </c>
-      <c r="J21" s="2">
-        <f t="shared" si="4"/>
+      <c r="K21" s="2">
+        <f>I20-I21</f>
         <v>15280.78594726033</v>
       </c>
     </row>
-    <row r="22" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E22" s="1">
         <v>21</v>
       </c>
@@ -1053,12 +1053,12 @@
         <f t="shared" si="3"/>
         <v>699666.39275667362</v>
       </c>
-      <c r="J22" s="2">
-        <f t="shared" si="4"/>
+      <c r="K22" s="2">
+        <f>I21-I22</f>
         <v>15395.391841864795</v>
       </c>
     </row>
-    <row r="23" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E23" s="1">
         <v>22</v>
       </c>
@@ -1078,12 +1078,12 @@
         <f t="shared" si="3"/>
         <v>684155.53547599481</v>
       </c>
-      <c r="J23" s="2">
-        <f t="shared" si="4"/>
+      <c r="K23" s="2">
+        <f>I22-I23</f>
         <v>15510.857280678814</v>
       </c>
     </row>
-    <row r="24" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E24" s="1">
         <v>23</v>
       </c>
@@ -1103,12 +1103,12 @@
         <f t="shared" si="3"/>
         <v>668528.34676571097</v>
       </c>
-      <c r="J24" s="2">
-        <f t="shared" si="4"/>
+      <c r="K24" s="2">
+        <f>I23-I24</f>
         <v>15627.188710283837</v>
       </c>
     </row>
-    <row r="25" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E25" s="1">
         <v>24</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>652783.95414009993</v>
       </c>
     </row>
-    <row r="26" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E26" s="1">
         <v>25</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>636921.47856979689</v>
       </c>
     </row>
-    <row r="27" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E27" s="1">
         <v>26</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>620940.03443271655</v>
       </c>
     </row>
-    <row r="28" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E28" s="1">
         <v>27</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>604838.72946460813</v>
       </c>
     </row>
-    <row r="29" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E29" s="1">
         <v>28</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>588616.66470923892</v>
       </c>
     </row>
-    <row r="30" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E30" s="1">
         <v>29</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>572272.93446820439</v>
       </c>
     </row>
-    <row r="31" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E31" s="1">
         <v>30</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>555806.62625036214</v>
       </c>
     </row>
-    <row r="32" spans="5:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E32" s="1">
         <v>31</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>33</v>
       </c>
       <c r="F34" s="2">
-        <f t="shared" ref="F34:F61" si="5">B$1*B$4/(1-(1+B$4)^-B$6)</f>
+        <f t="shared" ref="F34:F61" si="4">B$1*B$4/(1-(1+B$4)^-B$6)</f>
         <v>20758.355226353822</v>
       </c>
       <c r="G34" s="2">
@@ -1323,11 +1323,11 @@
         <v>34</v>
       </c>
       <c r="F35" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G35" s="2">
-        <f t="shared" ref="G35:G61" si="6">I34*B$4</f>
+        <f t="shared" ref="G35:G61" si="5">I34*B$4</f>
         <v>3792.4725439571962</v>
       </c>
       <c r="H35" s="2">
@@ -1344,11 +1344,11 @@
         <v>35</v>
       </c>
       <c r="F36" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G36" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3665.2284238392217</v>
       </c>
       <c r="H36" s="2">
@@ -1365,11 +1365,11 @@
         <v>36</v>
       </c>
       <c r="F37" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G37" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3537.0299728203622</v>
       </c>
       <c r="H37" s="2">
@@ -1386,11 +1386,11 @@
         <v>37</v>
       </c>
       <c r="F38" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G38" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3407.8700334188616</v>
       </c>
       <c r="H38" s="2">
@@ -1407,11 +1407,11 @@
         <v>38</v>
       </c>
       <c r="F39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G39" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3277.7413944718492</v>
       </c>
       <c r="H39" s="2">
@@ -1428,11 +1428,11 @@
         <v>39</v>
       </c>
       <c r="F40" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G40" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3146.6367907327344</v>
       </c>
       <c r="H40" s="2">
@@ -1449,11 +1449,11 @@
         <v>40</v>
       </c>
       <c r="F41" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G41" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3014.5489024655762</v>
       </c>
       <c r="H41" s="2">
@@ -1470,11 +1470,11 @@
         <v>41</v>
       </c>
       <c r="F42" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G42" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2881.4703550364147</v>
       </c>
       <c r="H42" s="2">
@@ -1491,11 +1491,11 @@
         <v>42</v>
       </c>
       <c r="F43" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G43" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2747.3937185015338</v>
       </c>
       <c r="H43" s="2">
@@ -1512,11 +1512,11 @@
         <v>43</v>
       </c>
       <c r="F44" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G44" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2612.3115071926418</v>
       </c>
       <c r="H44" s="2">
@@ -1533,11 +1533,11 @@
         <v>44</v>
       </c>
       <c r="F45" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G45" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2476.2161792989327</v>
       </c>
       <c r="H45" s="2">
@@ -1554,11 +1554,11 @@
         <v>45</v>
       </c>
       <c r="F46" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G46" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2339.1001364460212</v>
       </c>
       <c r="H46" s="2">
@@ -1575,11 +1575,11 @@
         <v>46</v>
       </c>
       <c r="F47" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G47" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2200.9557232717129</v>
       </c>
       <c r="H47" s="2">
@@ -1596,11 +1596,11 @@
         <v>47</v>
       </c>
       <c r="F48" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G48" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2061.7752269985972</v>
       </c>
       <c r="H48" s="2">
@@ -1617,11 +1617,11 @@
         <v>48</v>
       </c>
       <c r="F49" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G49" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1921.550877003433</v>
       </c>
       <c r="H49" s="2">
@@ -1638,11 +1638,11 @@
         <v>49</v>
       </c>
       <c r="F50" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G50" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1780.274844383305</v>
       </c>
       <c r="H50" s="2">
@@ -1659,11 +1659,11 @@
         <v>50</v>
       </c>
       <c r="F51" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G51" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1637.9392415185259</v>
       </c>
       <c r="H51" s="2">
@@ -1680,11 +1680,11 @@
         <v>51</v>
       </c>
       <c r="F52" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G52" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1494.5361216322613</v>
       </c>
       <c r="H52" s="2">
@@ -1701,11 +1701,11 @@
         <v>52</v>
       </c>
       <c r="F53" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G53" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1350.0574783468496</v>
       </c>
       <c r="H53" s="2">
@@ -1722,11 +1722,11 @@
         <v>53</v>
       </c>
       <c r="F54" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G54" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1204.4952452367972</v>
       </c>
       <c r="H54" s="2">
@@ -1743,11 +1743,11 @@
         <v>54</v>
       </c>
       <c r="F55" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G55" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1057.8412953784198</v>
       </c>
       <c r="H55" s="2">
@@ -1764,11 +1764,11 @@
         <v>55</v>
       </c>
       <c r="F56" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G56" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>910.08744089610423</v>
       </c>
       <c r="H56" s="2">
@@ -1785,11 +1785,11 @@
         <v>56</v>
       </c>
       <c r="F57" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G57" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>761.22543250517128</v>
       </c>
       <c r="H57" s="2">
@@ -1806,11 +1806,11 @@
         <v>57</v>
       </c>
       <c r="F58" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G58" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>611.24695905130636</v>
       </c>
       <c r="H58" s="2">
@@ -1827,11 +1827,11 @@
         <v>58</v>
       </c>
       <c r="F59" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G59" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>460.14364704653758</v>
       </c>
       <c r="H59" s="2">
@@ -1848,11 +1848,11 @@
         <v>59</v>
       </c>
       <c r="F60" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G60" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>307.90706020173297</v>
       </c>
       <c r="H60" s="2">
@@ -1869,11 +1869,11 @@
         <v>60</v>
       </c>
       <c r="F61" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20758.355226353822</v>
       </c>
       <c r="G61" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>154.52869895559229</v>
       </c>
       <c r="H61" s="2">
@@ -1895,12 +1895,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2062,15 +2059,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66699EEE-DA06-4892-8225-A3029FB87751}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64176B53-8F88-489E-9E50-82FD3C43066D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2094,10 +2095,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64176B53-8F88-489E-9E50-82FD3C43066D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66699EEE-DA06-4892-8225-A3029FB87751}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>